<commit_message>
adding ncbi upload files
</commit_message>
<xml_diff>
--- a/Raw_data/NCBI/Pacuta_HI_2022_Invertebrate.1.0.xlsx
+++ b/Raw_data/NCBI/Pacuta_HI_2022_Invertebrate.1.0.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="OGbkFCsCdx3Mx4gaQt2Jg11XPoZ2Uu8gbecS84tuTOU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="o9D9N4CKncCNXYozgQnMLohq2y5kAorEx0KrCnAsf3s="/>
     </ext>
   </extLst>
 </workbook>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="80">
   <si>
     <r>
       <rPr>
@@ -511,6 +511,9 @@
     <t>Medium</t>
   </si>
   <si>
+    <t>TreatmentReplicate</t>
+  </si>
+  <si>
     <t>AnalyzedBy</t>
   </si>
   <si>
@@ -523,6 +526,9 @@
     <t>A</t>
   </si>
   <si>
+    <t>A_Pacuta_High_20220718</t>
+  </si>
+  <si>
     <t>Pocillopora acuta</t>
   </si>
   <si>
@@ -532,7 +538,7 @@
     <t>Not applicable</t>
   </si>
   <si>
-    <t>18-Jul-22</t>
+    <t>2022-07-18</t>
   </si>
   <si>
     <t>USA: Kaneohe Bay Oahu Hawaii</t>
@@ -580,6 +586,9 @@
     <t>B</t>
   </si>
   <si>
+    <t>B_Pacuta_Control_20220718</t>
+  </si>
+  <si>
     <t>Control</t>
   </si>
   <si>
@@ -589,7 +598,13 @@
     <t>C</t>
   </si>
   <si>
+    <t>C_Pacuta_Control_20220718</t>
+  </si>
+  <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>D_Pacuta_Mid_20220718</t>
   </si>
   <si>
     <t>Mid</t>
@@ -601,22 +616,43 @@
     <t>E</t>
   </si>
   <si>
+    <t>E_Pacuta_Control_20220718</t>
+  </si>
+  <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>F_Pacuta_Mid_20220718</t>
   </si>
   <si>
     <t>G</t>
   </si>
   <si>
+    <t>G_Pacuta_Control_20220718</t>
+  </si>
+  <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>H_Pacuta_Mid_20220718</t>
   </si>
   <si>
     <t>L</t>
   </si>
   <si>
+    <t>L_Pacuta_High_20220718</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
+    <t>M_Pacuta_Mid_20220718</t>
+  </si>
+  <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>N_Pacuta_High_20220718</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1072,7 @@
     <col customWidth="1" min="15" max="15" width="21.71"/>
     <col customWidth="1" min="16" max="16" width="15.71"/>
     <col customWidth="1" min="17" max="17" width="9.71"/>
-    <col customWidth="1" min="18" max="23" width="8.71"/>
+    <col customWidth="1" min="18" max="24" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1065,6 +1101,7 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
@@ -1092,6 +1129,7 @@
       <c r="U2" s="3"/>
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
@@ -1119,6 +1157,7 @@
       <c r="U3" s="5"/>
       <c r="V3" s="5"/>
       <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
     </row>
     <row r="4">
       <c r="A4" s="6" t="s">
@@ -1146,6 +1185,7 @@
       <c r="U4" s="7"/>
       <c r="V4" s="7"/>
       <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
@@ -1173,6 +1213,7 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
@@ -1200,6 +1241,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
@@ -1227,6 +1269,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
     </row>
     <row r="8">
       <c r="A8" s="8" t="s">
@@ -1254,6 +1297,7 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
       <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
@@ -1281,6 +1325,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
@@ -1308,6 +1353,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
@@ -1335,6 +1381,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
@@ -1362,6 +1409,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
     </row>
     <row r="13">
       <c r="A13" s="9" t="s">
@@ -1433,742 +1481,800 @@
       <c r="W13" s="13" t="s">
         <v>34</v>
       </c>
+      <c r="X13" s="13" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B14" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>37</v>
+      </c>
       <c r="C14" s="15"/>
       <c r="D14" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I14" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N14" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O14" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P14" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q14" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R14" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S14" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T14" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="U14" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="U14" s="18">
+        <v>1.0</v>
       </c>
       <c r="V14" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W14" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W14" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X14" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>57</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K15" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L15" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N15" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P15" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q15" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R15" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T15" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="U15" s="18">
+        <v>1.0</v>
+      </c>
+      <c r="V15" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W15" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X15" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="T15" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="U15" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="V15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W15" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>61</v>
+      </c>
       <c r="C16" s="15"/>
       <c r="D16" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J16" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K16" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L16" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M16" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N16" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P16" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q16" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R16" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S16" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T16" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="U16" s="18">
+        <v>2.0</v>
+      </c>
+      <c r="V16" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W16" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X16" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="T16" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="U16" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="V16" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W16" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17" s="15"/>
+        <v>62</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>63</v>
+      </c>
       <c r="C17" s="15"/>
       <c r="D17" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J17" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K17" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M17" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N17" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O17" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P17" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q17" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R17" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S17" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="T17" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="U17" s="18" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="U17" s="18">
+        <v>1.0</v>
       </c>
       <c r="V17" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W17" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X17" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="15"/>
+        <v>66</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>67</v>
+      </c>
       <c r="C18" s="15"/>
       <c r="D18" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I18" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J18" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K18" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M18" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N18" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O18" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P18" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q18" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R18" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S18" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T18" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="U18" s="18">
+        <v>3.0</v>
+      </c>
+      <c r="V18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W18" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X18" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="T18" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="U18" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="V18" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W18" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="15"/>
+        <v>68</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="C19" s="15"/>
       <c r="D19" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I19" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J19" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K19" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M19" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N19" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P19" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q19" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R19" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S19" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="T19" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="U19" s="18" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="U19" s="18">
+        <v>2.0</v>
       </c>
       <c r="V19" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W19" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W19" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X19" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B20" s="15"/>
+        <v>70</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>71</v>
+      </c>
       <c r="C20" s="15"/>
       <c r="D20" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I20" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J20" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K20" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M20" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N20" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O20" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P20" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q20" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R20" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S20" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="T20" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="U20" s="18">
+        <v>4.0</v>
+      </c>
+      <c r="V20" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="W20" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X20" s="19" t="s">
         <v>55</v>
-      </c>
-      <c r="T20" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="U20" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="V20" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W20" s="19" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B21" s="15"/>
+        <v>72</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="C21" s="15"/>
       <c r="D21" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J21" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K21" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M21" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N21" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O21" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P21" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q21" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R21" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S21" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="T21" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="U21" s="18" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="U21" s="18">
+        <v>3.0</v>
       </c>
       <c r="V21" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W21" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W21" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X21" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="15"/>
+        <v>74</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>75</v>
+      </c>
       <c r="C22" s="15"/>
       <c r="D22" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L22" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N22" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P22" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q22" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R22" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S22" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="U22" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="U22" s="18">
+        <v>2.0</v>
       </c>
       <c r="V22" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W22" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W22" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X22" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" s="15"/>
+        <v>76</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>77</v>
+      </c>
       <c r="C23" s="15"/>
       <c r="D23" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M23" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N23" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O23" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P23" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q23" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R23" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S23" s="18" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="T23" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="U23" s="18" t="s">
-        <v>51</v>
+        <v>65</v>
+      </c>
+      <c r="U23" s="18">
+        <v>4.0</v>
       </c>
       <c r="V23" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W23" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W23" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X23" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="15"/>
+        <v>78</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>79</v>
+      </c>
       <c r="C24" s="15"/>
       <c r="D24" s="14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J24" s="16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="K24" s="17" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="M24" s="14" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="N24" s="17" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="O24" s="14" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="P24" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q24" s="17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R24" s="18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="S24" s="18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="T24" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="U24" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="U24" s="18">
+        <v>3.0</v>
       </c>
       <c r="V24" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="W24" s="19" t="s">
         <v>53</v>
+      </c>
+      <c r="W24" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="X24" s="19" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">

</xml_diff>